<commit_message>
double move test. find possible moves fixed
</commit_message>
<xml_diff>
--- a/rows_columns_excel.xlsx
+++ b/rows_columns_excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\Studie\CS - Module 2\TCSM2-Programming-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emiel\Documents\Studie\CS - Module 2\TCSM2-Programming-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CD7E1CB-7646-4A14-BDBA-8E752FAFCFB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E3852B-9FA4-453B-A360-178192B8A3B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1785" windowWidth="13290" windowHeight="15480" xr2:uid="{1A374059-226A-4C88-820A-6A33DEE53B95}"/>
+    <workbookView xWindow="-5580" yWindow="6015" windowWidth="13920" windowHeight="15420" xr2:uid="{1A374059-226A-4C88-820A-6A33DEE53B95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,16 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>ß</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98CC35F7-F6BD-4D50-88F1-99AC250712CF}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,8 +759,8 @@
       <c r="A8" s="5">
         <v>14</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>0</v>
+      <c r="B8" s="17">
+        <v>42</v>
       </c>
       <c r="C8" s="9">
         <v>43</v>
@@ -800,6 +805,59 @@
       </c>
       <c r="H9" s="3">
         <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5">
+        <v>4</v>
+      </c>
+      <c r="G10" s="5">
+        <v>5</v>
+      </c>
+      <c r="H10" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <f>21-3*7</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <f xml:space="preserve"> 2 * 7 - 12-1</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
+        <f xml:space="preserve"> 2 * 7 - 11 -1</f>
+        <v>2</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" ref="E11:H11" si="0" xml:space="preserve"> 2 * 7 - 12-1</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" ref="F11:H11" si="1" xml:space="preserve"> 2 * 7 - 13 -1</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" ref="G11:H11" si="2" xml:space="preserve"> 2 * 7 - 12-1</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" ref="H11" si="3" xml:space="preserve"> 2 * 7 - 13 -1</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created most of the gui. added chatbox functionality
</commit_message>
<xml_diff>
--- a/rows_columns_excel.xlsx
+++ b/rows_columns_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emiel\Documents\Studie\CS - Module 2\TCSM2-Programming-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E3852B-9FA4-453B-A360-178192B8A3B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4D9E2B-A7AA-44A7-954F-34012CDC3000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5580" yWindow="6015" windowWidth="13920" windowHeight="15420" xr2:uid="{1A374059-226A-4C88-820A-6A33DEE53B95}"/>
+    <workbookView xWindow="-5805" yWindow="600" windowWidth="13920" windowHeight="15420" xr2:uid="{1A374059-226A-4C88-820A-6A33DEE53B95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>21;6</t>
+  </si>
+  <si>
+    <t>21;14</t>
+  </si>
+  <si>
+    <t>6;13</t>
+  </si>
+  <si>
+    <t>6;21</t>
+  </si>
+  <si>
+    <t>20;26</t>
+  </si>
+  <si>
+    <t>7;1</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,13 +68,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -64,7 +90,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -175,15 +206,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -196,45 +225,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Accent6" xfId="1" builtinId="49"/>
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -547,317 +553,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98CC35F7-F6BD-4D50-88F1-99AC250712CF}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="5">
+    <row r="1" spans="1:16" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="4">
         <v>21</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1" s="4">
         <v>22</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="4">
         <v>23</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1" s="4">
         <v>24</v>
       </c>
-      <c r="F1" s="5">
+      <c r="F1" s="4">
         <v>25</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="4">
         <v>26</v>
       </c>
-      <c r="H1" s="5">
+      <c r="H1" s="4">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+    <row r="2" spans="1:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>20</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="5">
         <v>0</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="6">
         <v>2</v>
       </c>
       <c r="E2" s="6">
         <v>3</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="6">
         <v>4</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="6">
         <v>5</v>
       </c>
       <c r="H2" s="13">
         <v>6</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="L2" s="4">
+        <v>20</v>
+      </c>
+      <c r="M2" s="4">
+        <v>27</v>
+      </c>
+      <c r="O2" s="4">
+        <v>6</v>
+      </c>
+      <c r="P2" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>19</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="7">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="8">
         <v>8</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="8">
         <v>9</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="8">
         <v>10</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="8">
         <v>11</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="8">
         <v>12</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="9">
         <v>13</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="L3" s="4">
+        <v>20</v>
+      </c>
+      <c r="M3" s="4">
+        <v>7</v>
+      </c>
+      <c r="O3" s="4">
+        <v>6</v>
+      </c>
+      <c r="P3" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>18</v>
       </c>
       <c r="B4" s="7">
         <v>14</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="8">
         <v>15</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="8">
         <v>16</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="8">
         <v>17</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="8">
         <v>18</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="8">
         <v>19</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="9">
         <v>20</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="L4" s="4">
+        <v>21</v>
+      </c>
+      <c r="M4" s="4">
+        <v>14</v>
+      </c>
+      <c r="O4" s="4">
+        <v>7</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>17</v>
       </c>
       <c r="B5" s="7">
         <v>21</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="8">
         <v>22</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="8">
         <v>23</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="8">
         <v>24</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="8">
         <v>25</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="8">
         <v>26</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="9">
         <v>27</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="L5" s="4">
+        <v>21</v>
+      </c>
+      <c r="M5" s="4">
+        <v>6</v>
+      </c>
+      <c r="O5" s="4">
+        <v>7</v>
+      </c>
+      <c r="P5" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>16</v>
       </c>
       <c r="B6" s="7">
         <v>28</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="8">
         <v>29</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="8">
         <v>30</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="8">
         <v>31</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="8">
         <v>32</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="8">
         <v>33</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="9">
         <v>34</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>15</v>
       </c>
       <c r="B7" s="7">
         <v>35</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="8">
         <v>36</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="8">
         <v>37</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="8">
         <v>38</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="8">
         <v>39</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="8">
         <v>40</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="9">
         <v>41</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+    <row r="8" spans="1:16" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>14</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="10">
         <v>42</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="11">
         <v>43</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="11">
         <v>44</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="11">
         <v>45</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="11">
         <v>46</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="11">
         <v>47</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="12">
         <v>48</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
+    <row r="9" spans="1:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
         <v>13</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>12</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>11</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>10</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>9</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>8</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5">
-        <v>2</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="5">
-        <v>4</v>
-      </c>
-      <c r="G10" s="5">
+      <c r="D11" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="H10" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="5">
-        <f>21-3*7</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="5">
-        <f xml:space="preserve"> 2 * 7 - 12-1</f>
-        <v>1</v>
-      </c>
-      <c r="D11" s="5">
-        <f xml:space="preserve"> 2 * 7 - 11 -1</f>
-        <v>2</v>
-      </c>
-      <c r="E11" s="5">
-        <f t="shared" ref="E11:H11" si="0" xml:space="preserve"> 2 * 7 - 12-1</f>
-        <v>1</v>
-      </c>
-      <c r="F11" s="5">
-        <f t="shared" ref="F11:H11" si="1" xml:space="preserve"> 2 * 7 - 13 -1</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="5">
-        <f t="shared" ref="G11:H11" si="2" xml:space="preserve"> 2 * 7 - 12-1</f>
-        <v>1</v>
-      </c>
-      <c r="H11" s="5">
-        <f t="shared" ref="H11" si="3" xml:space="preserve"> 2 * 7 - 13 -1</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>